<commit_message>
set font-size for proper display in Survey app
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bennett\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bennett\workspace\cse481k\AdaptiveODK\form-files\adaptiveIMCI_community\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="515">
   <si>
     <t>type</t>
   </si>
@@ -1562,6 +1562,12 @@
   </si>
   <si>
     <t>Community Version</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>11pt</t>
   </si>
 </sst>
 </file>
@@ -55281,11 +55287,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -55350,14 +55356,12 @@
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="A7" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>514</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleanup, hacked jump to demographics page (menu.handlebars)
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9564" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2009,32 +2009,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="41" style="3" customWidth="1"/>
     <col min="6" max="6" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="3"/>
-    <col min="8" max="8" width="20.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" style="3" customWidth="1"/>
-    <col min="10" max="12" width="8.88671875" style="3"/>
-    <col min="13" max="13" width="17.33203125" style="3" customWidth="1"/>
-    <col min="14" max="15" width="8.88671875" style="3"/>
-    <col min="16" max="16" width="17.44140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="19.88671875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="21.5546875" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="8.85546875" style="3"/>
+    <col min="8" max="8" width="20.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="3" customWidth="1"/>
+    <col min="10" max="12" width="8.85546875" style="3"/>
+    <col min="13" max="13" width="17.28515625" style="3" customWidth="1"/>
+    <col min="14" max="15" width="8.85546875" style="3"/>
+    <col min="16" max="16" width="17.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>140</v>
       </c>
@@ -2115,7 +2115,7 @@
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -2139,7 +2139,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -2180,7 +2180,9 @@
         <v>42</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="13"/>
@@ -2193,7 +2195,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -2219,7 +2221,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -2247,7 +2249,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -2269,7 +2271,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
@@ -2291,7 +2293,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>43</v>
       </c>
@@ -2315,7 +2317,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -2345,7 +2347,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -2375,7 +2377,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -2405,7 +2407,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
@@ -2427,7 +2429,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>43</v>
       </c>
@@ -2451,7 +2453,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -2480,7 +2482,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
@@ -2510,7 +2512,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -2540,7 +2542,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
@@ -2570,7 +2572,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
@@ -2592,7 +2594,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>142</v>
       </c>
@@ -2614,7 +2616,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>43</v>
       </c>
@@ -2640,7 +2642,7 @@
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>153</v>
       </c>
@@ -2668,7 +2670,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>153</v>
       </c>
@@ -2694,7 +2696,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
@@ -2722,7 +2724,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
@@ -2744,7 +2746,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>157</v>
       </c>
@@ -2765,7 +2767,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>43</v>
       </c>
@@ -2791,7 +2793,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>153</v>
       </c>
@@ -2819,7 +2821,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>24</v>
       </c>
@@ -2847,7 +2849,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -2875,7 +2877,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -2903,7 +2905,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
@@ -2931,7 +2933,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
@@ -2959,7 +2961,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
@@ -2987,7 +2989,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
@@ -3015,7 +3017,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>48</v>
       </c>
@@ -3037,7 +3039,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>200</v>
       </c>
@@ -3058,7 +3060,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>43</v>
       </c>
@@ -3084,7 +3086,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -3112,7 +3114,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>153</v>
       </c>
@@ -3140,7 +3142,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>24</v>
       </c>
@@ -3168,7 +3170,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>24</v>
       </c>
@@ -3196,7 +3198,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>24</v>
       </c>
@@ -3224,7 +3226,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>24</v>
       </c>
@@ -3252,7 +3254,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>48</v>
       </c>
@@ -3274,7 +3276,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>43</v>
       </c>
@@ -3300,7 +3302,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>24</v>
       </c>
@@ -3328,7 +3330,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>24</v>
       </c>
@@ -3356,7 +3358,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>24</v>
       </c>
@@ -3384,7 +3386,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>48</v>
       </c>
@@ -3406,7 +3408,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>143</v>
       </c>
@@ -3428,7 +3430,7 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>43</v>
       </c>
@@ -3451,7 +3453,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>24</v>
       </c>
@@ -3479,7 +3481,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>24</v>
       </c>
@@ -3507,7 +3509,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>24</v>
       </c>
@@ -3535,7 +3537,7 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>24</v>
       </c>
@@ -3563,7 +3565,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>48</v>
       </c>
@@ -3585,7 +3587,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>194</v>
       </c>
@@ -3607,7 +3609,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>43</v>
       </c>
@@ -3630,7 +3632,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>24</v>
       </c>
@@ -3658,7 +3660,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>24</v>
       </c>
@@ -3686,7 +3688,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>24</v>
       </c>
@@ -3714,7 +3716,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>24</v>
       </c>
@@ -3742,7 +3744,7 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
@@ -3772,7 +3774,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>48</v>
       </c>
@@ -3794,7 +3796,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>31</v>
       </c>
@@ -3822,7 +3824,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>43</v>
       </c>
@@ -3848,7 +3850,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>228</v>
       </c>
@@ -3874,7 +3876,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>228</v>
       </c>
@@ -3900,7 +3902,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>233</v>
       </c>
@@ -3927,7 +3929,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>228</v>
       </c>
@@ -3953,7 +3955,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>239</v>
       </c>
@@ -3980,7 +3982,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>48</v>
       </c>
@@ -4002,28 +4004,28 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
       <c r="D82" s="16"/>
       <c r="E82" s="17"/>
       <c r="F82" s="17"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="16"/>
       <c r="D83" s="16"/>
       <c r="E83" s="17"/>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="16"/>
       <c r="D84" s="16"/>
       <c r="E84" s="17"/>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="16"/>
       <c r="D85" s="16"/>
       <c r="E85" s="17"/>
@@ -4044,14 +4046,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="17.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -4073,14 +4075,14 @@
       <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
-    <col min="2" max="2" width="97.44140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="97.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -4088,8 +4090,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -4097,7 +4099,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
@@ -4105,7 +4107,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>202</v>
       </c>
@@ -4113,7 +4115,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
@@ -4121,7 +4123,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
@@ -4129,7 +4131,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -4137,7 +4139,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
@@ -4145,7 +4147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
@@ -4153,7 +4155,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -4161,7 +4163,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -4169,7 +4171,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -4177,7 +4179,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>204</v>
       </c>
@@ -4185,7 +4187,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>207</v>
       </c>
@@ -4193,7 +4195,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>210</v>
       </c>
@@ -4201,7 +4203,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>212</v>
       </c>
@@ -4209,7 +4211,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>214</v>
       </c>
@@ -4217,7 +4219,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -4225,7 +4227,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>318</v>
       </c>
@@ -4233,7 +4235,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>319</v>
       </c>
@@ -4241,7 +4243,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>320</v>
       </c>
@@ -4249,7 +4251,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>215</v>
       </c>
@@ -4257,7 +4259,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>328</v>
       </c>
@@ -4265,7 +4267,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>266</v>
       </c>
@@ -4273,7 +4275,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>217</v>
       </c>
@@ -4281,7 +4283,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>219</v>
       </c>
@@ -4289,7 +4291,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
@@ -4297,7 +4299,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>220</v>
       </c>
@@ -4305,7 +4307,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="35" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>221</v>
       </c>
@@ -4313,7 +4315,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="36" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>275</v>
       </c>
@@ -20703,7 +20705,7 @@
       <c r="XFC36" s="4"/>
       <c r="XFD36" s="4"/>
     </row>
-    <row r="37" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>276</v>
       </c>
@@ -37093,7 +37095,7 @@
       <c r="XFC37" s="4"/>
       <c r="XFD37" s="4"/>
     </row>
-    <row r="38" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>277</v>
       </c>
@@ -53483,7 +53485,7 @@
       <c r="XFC38" s="4"/>
       <c r="XFD38" s="4"/>
     </row>
-    <row r="40" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
@@ -53491,7 +53493,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
@@ -53499,7 +53501,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -53507,7 +53509,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>333</v>
       </c>
@@ -53515,7 +53517,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="45" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>222</v>
       </c>
@@ -53523,7 +53525,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="46" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>223</v>
       </c>
@@ -53531,7 +53533,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="47" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>224</v>
       </c>
@@ -53539,7 +53541,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="48" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>225</v>
       </c>
@@ -53547,7 +53549,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>403</v>
       </c>
@@ -53555,7 +53557,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>463</v>
       </c>
@@ -53563,7 +53565,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>92</v>
       </c>
@@ -53571,7 +53573,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>101</v>
       </c>
@@ -53579,7 +53581,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>94</v>
       </c>
@@ -53587,7 +53589,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>98</v>
       </c>
@@ -53595,7 +53597,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>96</v>
       </c>
@@ -53603,7 +53605,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>198</v>
       </c>
@@ -53611,7 +53613,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>99</v>
       </c>
@@ -53619,7 +53621,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>100</v>
       </c>
@@ -53627,7 +53629,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
@@ -53635,7 +53637,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -53643,7 +53645,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -53651,7 +53653,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>196</v>
       </c>
@@ -53659,7 +53661,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>242</v>
       </c>
@@ -53667,7 +53669,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>249</v>
       </c>
@@ -53675,7 +53677,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>264</v>
       </c>
@@ -53683,7 +53685,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>295</v>
       </c>
@@ -53691,7 +53693,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>271</v>
       </c>
@@ -53699,7 +53701,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>272</v>
       </c>
@@ -53707,7 +53709,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>273</v>
       </c>
@@ -53715,7 +53717,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>306</v>
       </c>
@@ -53723,7 +53725,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>296</v>
       </c>
@@ -53731,7 +53733,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>297</v>
       </c>
@@ -53739,7 +53741,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>298</v>
       </c>
@@ -53747,7 +53749,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>373</v>
       </c>
@@ -53755,7 +53757,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>375</v>
       </c>
@@ -53763,7 +53765,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>377</v>
       </c>
@@ -53771,7 +53773,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>379</v>
       </c>
@@ -53779,7 +53781,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>381</v>
       </c>
@@ -53787,7 +53789,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>383</v>
       </c>
@@ -53795,7 +53797,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>385</v>
       </c>
@@ -53803,7 +53805,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>386</v>
       </c>
@@ -53811,7 +53813,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>387</v>
       </c>
@@ -53819,7 +53821,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>388</v>
       </c>
@@ -53827,7 +53829,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>381</v>
       </c>
@@ -53835,7 +53837,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>389</v>
       </c>
@@ -53843,7 +53845,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>308</v>
       </c>
@@ -53851,7 +53853,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>325</v>
       </c>
@@ -53859,7 +53861,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>329</v>
       </c>
@@ -53867,7 +53869,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>299</v>
       </c>
@@ -53875,7 +53877,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>300</v>
       </c>
@@ -53883,7 +53885,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>330</v>
       </c>
@@ -53891,7 +53893,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>301</v>
       </c>
@@ -53899,7 +53901,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>302</v>
       </c>
@@ -53907,7 +53909,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>303</v>
       </c>
@@ -53915,7 +53917,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>304</v>
       </c>
@@ -53923,7 +53925,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>305</v>
       </c>
@@ -53931,7 +53933,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>405</v>
       </c>
@@ -53939,7 +53941,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>406</v>
       </c>
@@ -53961,19 +53963,19 @@
       <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.44140625" customWidth="1"/>
-    <col min="8" max="8" width="44.88671875" customWidth="1"/>
-    <col min="9" max="9" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.42578125" customWidth="1"/>
+    <col min="8" max="8" width="44.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -54005,7 +54007,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -54022,7 +54024,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -54039,7 +54041,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -54064,7 +54066,7 @@
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -54089,7 +54091,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
@@ -54114,7 +54116,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -54139,7 +54141,7 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
@@ -54164,7 +54166,7 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
@@ -54187,7 +54189,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -54196,7 +54198,7 @@
       <c r="F10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>240</v>
       </c>
@@ -54213,13 +54215,13 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>240</v>
       </c>
@@ -54236,7 +54238,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>240</v>
       </c>
@@ -54253,7 +54255,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>240</v>
       </c>
@@ -54270,7 +54272,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>240</v>
       </c>
@@ -54287,7 +54289,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>240</v>
       </c>
@@ -54304,7 +54306,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>240</v>
       </c>
@@ -54321,7 +54323,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>240</v>
       </c>
@@ -54338,13 +54340,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>240</v>
       </c>
@@ -54361,7 +54363,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>240</v>
       </c>
@@ -54378,7 +54380,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>240</v>
       </c>
@@ -54395,7 +54397,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>240</v>
       </c>
@@ -54412,7 +54414,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>240</v>
       </c>
@@ -54429,13 +54431,13 @@
         <v>293</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>240</v>
       </c>
@@ -54452,7 +54454,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>240</v>
       </c>
@@ -54469,13 +54471,13 @@
         <v>350</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>240</v>
       </c>
@@ -54492,7 +54494,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>240</v>
       </c>
@@ -54509,7 +54511,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>240</v>
       </c>
@@ -54526,7 +54528,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>240</v>
       </c>
@@ -54543,7 +54545,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>240</v>
       </c>
@@ -54560,7 +54562,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>240</v>
       </c>
@@ -54577,7 +54579,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>240</v>
       </c>
@@ -54594,13 +54596,13 @@
         <v>476</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>240</v>
       </c>
@@ -54617,13 +54619,13 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>240</v>
       </c>
@@ -54640,13 +54642,13 @@
         <v>355</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>240</v>
       </c>
@@ -54663,7 +54665,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>240</v>
       </c>
@@ -54680,7 +54682,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>240</v>
       </c>
@@ -54697,13 +54699,13 @@
         <v>357</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>240</v>
       </c>
@@ -54720,13 +54722,13 @@
         <v>412</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>247</v>
       </c>
@@ -54740,7 +54742,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>247</v>
       </c>
@@ -54754,7 +54756,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>247</v>
       </c>
@@ -54768,12 +54770,12 @@
         <v>505</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>247</v>
       </c>
@@ -54790,7 +54792,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>247</v>
       </c>
@@ -54805,7 +54807,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>247</v>
       </c>
@@ -54820,7 +54822,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>247</v>
       </c>
@@ -54835,7 +54837,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>247</v>
       </c>
@@ -54850,7 +54852,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>247</v>
       </c>
@@ -54864,7 +54866,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>247</v>
       </c>
@@ -54878,7 +54880,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>247</v>
       </c>
@@ -54892,7 +54894,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>247</v>
       </c>
@@ -54907,7 +54909,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>247</v>
       </c>
@@ -54922,7 +54924,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>247</v>
       </c>
@@ -54937,7 +54939,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>247</v>
       </c>
@@ -54951,7 +54953,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>247</v>
       </c>
@@ -54965,7 +54967,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>247</v>
       </c>
@@ -54980,7 +54982,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>247</v>
       </c>
@@ -54995,7 +54997,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>247</v>
       </c>
@@ -55010,7 +55012,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>247</v>
       </c>
@@ -55025,7 +55027,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>247</v>
       </c>
@@ -55040,7 +55042,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>247</v>
       </c>
@@ -55055,7 +55057,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>247</v>
       </c>
@@ -55070,7 +55072,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>247</v>
       </c>
@@ -55085,7 +55087,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>247</v>
       </c>
@@ -55100,7 +55102,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>247</v>
       </c>
@@ -55115,7 +55117,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>484</v>
       </c>
@@ -55130,7 +55132,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>484</v>
       </c>
@@ -55145,7 +55147,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>484</v>
       </c>
@@ -55160,7 +55162,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>484</v>
       </c>
@@ -55175,7 +55177,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>247</v>
       </c>
@@ -55190,7 +55192,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>247</v>
       </c>
@@ -55205,7 +55207,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>247</v>
       </c>
@@ -55220,7 +55222,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>247</v>
       </c>
@@ -55235,7 +55237,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>247</v>
       </c>
@@ -55250,7 +55252,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>247</v>
       </c>
@@ -55265,7 +55267,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>247</v>
       </c>
@@ -55289,19 +55291,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" style="5" customWidth="1"/>
     <col min="2" max="2" width="24" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="5"/>
+    <col min="3" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -55310,7 +55312,7 @@
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>17</v>
       </c>
@@ -55319,7 +55321,7 @@
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>508</v>
       </c>
@@ -55328,7 +55330,7 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
@@ -55337,7 +55339,7 @@
       </c>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
@@ -55346,7 +55348,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>511</v>
       </c>
@@ -55355,7 +55357,7 @@
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>513</v>
       </c>

</xml_diff>

<commit_message>
integrated updated Treatment info (Mariana
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="prompt_types" sheetId="5" r:id="rId2"/>
-    <sheet name="calculates" sheetId="2" r:id="rId3"/>
-    <sheet name="choices" sheetId="3" r:id="rId4"/>
-    <sheet name="settings" sheetId="4" r:id="rId5"/>
+    <sheet name="calculates" sheetId="2" r:id="rId2"/>
+    <sheet name="choices" sheetId="3" r:id="rId3"/>
+    <sheet name="settings" sheetId="4" r:id="rId4"/>
+    <sheet name="prompt_types" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="522">
   <si>
     <t>type</t>
   </si>
@@ -772,12 +772,6 @@
     <t>Give Quinine for severe Malaria (first dose)</t>
   </si>
   <si>
-    <t>Give first dose of antibiotic</t>
-  </si>
-  <si>
-    <t>Treat child to preven low blood sugar</t>
-  </si>
-  <si>
     <t>Give one dose of paracetamol in clinic for high fever (38.5 C or above)</t>
   </si>
   <si>
@@ -872,9 +866,6 @@
   </si>
   <si>
     <t>malaria_high</t>
-  </si>
-  <si>
-    <t>malaria_low</t>
   </si>
   <si>
     <t>measles_high</t>
@@ -1027,9 +1018,6 @@
     <t>(calculates.has_ear_problem() &amp;&amp; calculates.high_danger_ear() == "good" &amp;&amp; (calculates.has_ear_discharge() || calculates.has_ear_pain())) ? "danger" : "good"</t>
   </si>
   <si>
-    <t>pneumonia_high</t>
-  </si>
-  <si>
     <t>pneumonia_med</t>
   </si>
   <si>
@@ -1054,13 +1042,7 @@
     <t>dysentry</t>
   </si>
   <si>
-    <t>ear_high</t>
-  </si>
-  <si>
     <t>ear_med</t>
-  </si>
-  <si>
-    <t>{{calculates.high_danger_pneumonia()}}</t>
   </si>
   <si>
     <t>{{calculates.med_danger_pneumonia()}}</t>
@@ -1258,12 +1240,6 @@
     <t>{{calculates.med_danger_anemia()}}</t>
   </si>
   <si>
-    <t>Give first dose of appropriate antibiotic</t>
-  </si>
-  <si>
-    <t>due to severe pneumonia</t>
-  </si>
-  <si>
     <t>Give oral antibiotic for 3 days</t>
   </si>
   <si>
@@ -1321,13 +1297,7 @@
     <t>ear_med2</t>
   </si>
   <si>
-    <t>ear_med3</t>
-  </si>
-  <si>
     <t>Dry the ear by wicking</t>
-  </si>
-  <si>
-    <t>Follow up in 5 days</t>
   </si>
   <si>
     <t>Follow up in 5 days if not improving</t>
@@ -1354,9 +1324,6 @@
     <t>due to very severe febrile disease</t>
   </si>
   <si>
-    <t>due to fever</t>
-  </si>
-  <si>
     <t>malaria_med3</t>
   </si>
   <si>
@@ -1364,9 +1331,6 @@
   </si>
   <si>
     <t>malaria_low3</t>
-  </si>
-  <si>
-    <t>measles_high2</t>
   </si>
   <si>
     <t>measles_high3</t>
@@ -1447,16 +1411,10 @@
     <t>Give fluid, zinc supplements, and food for some dehydration</t>
   </si>
   <si>
-    <t>dehydration_med3</t>
-  </si>
-  <si>
     <t>due to some dehydration</t>
   </si>
   <si>
     <t>Give fluid, zinc supplements, and food to treat diarrhea at home</t>
-  </si>
-  <si>
-    <t>dehydration_low3</t>
   </si>
   <si>
     <t>Treat dehydration before referral unless the child has another severe classification</t>
@@ -1475,9 +1433,6 @@
   </si>
   <si>
     <t>diarrhea_med2</t>
-  </si>
-  <si>
-    <t>diarrhea_med3</t>
   </si>
   <si>
     <t>Give ciprofloxacin for 3 days</t>
@@ -1520,9 +1475,6 @@
   </si>
   <si>
     <t>anemia_med5</t>
-  </si>
-  <si>
-    <t>{{calculates.severe_classification()}}</t>
   </si>
   <si>
     <t>{{calculates.med_danger_dehydration() }}</t>
@@ -1599,12 +1551,51 @@
   <si>
     <t>submenu</t>
   </si>
+  <si>
+    <t>{{calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_ear() == "danger" ? "danger" : "good" }}</t>
+  </si>
+  <si>
+    <t>Treat child to prevent low blood sugar</t>
+  </si>
+  <si>
+    <t>{{calculates.high_danger_malaria() == "danger" || calculates.med_danger_malaria() == "danger" || calculates.low_danger_malaria() == "danger" ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>no_treat_now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of your child's ailments require immediate action. </t>
+  </si>
+  <si>
+    <t>{{calculates.danger_class_see_dr() != "danger" &amp;&amp; calculates.high_danger_malaria() != "danger" &amp;&amp; calculates.med_danger_malaria() != "danger" &amp;&amp; calculates.low_danger_malaria() != "danger" &amp;&amp; calculates.high_danger_measles() != "danger" &amp;&amp; calculates.med_danger_measles() != "danger" &amp;&amp; calculates.high_danger_pneumonia() != "danger" &amp;&amp; calculates.med_danger_pneumonia() != "danger" &amp;&amp; (calculates.high_danger_dehydration() != "danger" || calculates.severe_classification() != "good") &amp;&amp; (calculates.med_danger_dehydration() != "danger" || calculates.severe_classification() != "good") &amp;&amp; calculates.high_danger_diarrhea() != "danger" &amp;&amp; calculates.danger_dysentry() != "danger" &amp;&amp; calculates.high_danger_ear() != "danger" &amp;&amp; calculates.med_danger_ear() != "danger" &amp;&amp; calculates.high_danger_malnut() != "danger" ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>{{calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger" ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>{{!(calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger") &amp;&amp; (calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger")  ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>{{(calculates.low_danger_pneumonia() == "danger" || calculates.med_danger_dehydration() == "danger" || calculates.med_danger_ear() == "danger" || calculates.low_danger_dehydration() == "danger" || calculates.med_danger_diarrhea() == "danger") &amp;&amp; !(calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger"  || calculates.med_danger_malaria() == "danger" || calculates.low_danger_malaria() == "danger") ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>{{calculates.med_danger_malaria() == "danger" &amp;&amp; !(calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger") ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>{{calculates.low_danger_malaria() &amp;&amp; !( calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger"  ) ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>{{calculates.med_danger_malnut() == "danger" &amp;&amp; !(calculates.med_danger_anemia() == "danger" || calculates.low_danger_pneumonia() == "danger" || calculates.med_danger_dehydration() == "danger" || calculates.med_danger_ear() == "danger" || calculates.low_danger_dehydration() == "danger" || calculates.med_danger_diarrhea() == "danger" ||calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger"  || calculates.med_danger_malaria() == "danger" || calculates.low_danger_malaria() == "danger") ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>{{calculates.med_danger_anemia() == "danger" &amp;&amp; !(calculates.low_danger_pneumonia() == "danger" || calculates.med_danger_dehydration() == "danger" || calculates.med_danger_ear() == "danger" || calculates.low_danger_dehydration() == "danger" || calculates.med_danger_diarrhea() == "danger" || calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger"|| calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger"  || calculates.med_danger_malaria() == "danger" || calculates.low_danger_malaria() == "danger") ? "danger" : "good"}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1654,13 +1645,6 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1742,20 +1726,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1765,23 +1745,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -2070,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
@@ -2095,62 +2078,62 @@
     <col min="19" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="7" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2158,23 +2141,23 @@
       <c r="A2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2201,18 +2184,18 @@
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="4" t="b">
         <v>1</v>
       </c>
@@ -2246,7 +2229,7 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="13"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -2260,7 +2243,7 @@
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
         <v>44</v>
@@ -2271,8 +2254,8 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -2333,8 +2316,8 @@
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>514</v>
+      <c r="A9" s="18" t="s">
+        <v>498</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2377,7 +2360,7 @@
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2513,7 +2496,7 @@
       <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2678,8 +2661,8 @@
       <c r="R21" s="4"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>511</v>
+      <c r="A22" s="18" t="s">
+        <v>495</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2700,12 +2683,12 @@
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>520</v>
+      <c r="A23" s="20" t="s">
+        <v>504</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="21" t="s">
-        <v>517</v>
+      <c r="C23" s="19" t="s">
+        <v>501</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -2745,35 +2728,35 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>141</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="15"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="1" t="s">
         <v>203</v>
       </c>
@@ -2801,7 +2784,7 @@
         <v>152</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="15"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="4" t="s">
         <v>153</v>
       </c>
@@ -2827,7 +2810,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="15"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="1" t="s">
         <v>206</v>
       </c>
@@ -2855,7 +2838,7 @@
         <v>48</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="15"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2873,11 +2856,11 @@
       <c r="R29" s="4"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>512</v>
+      <c r="A30" s="18" t="s">
+        <v>496</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="15"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2895,12 +2878,12 @@
       <c r="R30" s="4"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>521</v>
+      <c r="A31" s="20" t="s">
+        <v>505</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="1" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2940,7 +2923,7 @@
       <c r="R32" s="4"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -2952,7 +2935,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="13"/>
+      <c r="J33" s="11"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -2967,7 +2950,7 @@
         <v>152</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="15"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="1" t="s">
         <v>208</v>
       </c>
@@ -3025,10 +3008,10 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>149</v>
@@ -3053,10 +3036,10 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>149</v>
@@ -3081,10 +3064,10 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>149</v>
@@ -3109,10 +3092,10 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>149</v>
@@ -3137,10 +3120,10 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>149</v>
@@ -3209,8 +3192,8 @@
       <c r="R42" s="4"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>513</v>
+      <c r="A43" s="18" t="s">
+        <v>497</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3231,12 +3214,12 @@
       <c r="R43" s="4"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
-        <v>522</v>
+      <c r="A44" s="20" t="s">
+        <v>506</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="1" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -3276,7 +3259,7 @@
       <c r="R45" s="4"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -3288,7 +3271,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="13"/>
+      <c r="J46" s="11"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
@@ -3305,10 +3288,10 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>149</v>
@@ -3316,7 +3299,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="13"/>
+      <c r="J47" s="11"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
@@ -3331,7 +3314,7 @@
         <v>152</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="15"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="1" t="s">
         <v>213</v>
       </c>
@@ -3359,7 +3342,7 @@
         <v>24</v>
       </c>
       <c r="B49" s="4"/>
-      <c r="C49" s="15"/>
+      <c r="C49" s="13"/>
       <c r="D49" s="4" t="s">
         <v>170</v>
       </c>
@@ -3489,7 +3472,7 @@
       <c r="R53" s="4"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -3504,7 +3487,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="13"/>
+      <c r="J54" s="11"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
@@ -3524,7 +3507,7 @@
         <v>175</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>149</v>
@@ -3621,8 +3604,8 @@
       <c r="R58" s="4"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
-        <v>523</v>
+      <c r="A59" s="18" t="s">
+        <v>507</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3665,7 +3648,7 @@
       <c r="R60" s="4"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -3677,7 +3660,7 @@
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
-      <c r="J61" s="13"/>
+      <c r="J61" s="11"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -3750,10 +3733,10 @@
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>149</v>
@@ -3822,8 +3805,8 @@
       <c r="R66" s="4"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
-        <v>515</v>
+      <c r="A67" s="18" t="s">
+        <v>499</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3866,7 +3849,7 @@
       <c r="R68" s="4"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -3878,7 +3861,7 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="13"/>
+      <c r="J69" s="11"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
@@ -4004,15 +3987,15 @@
       <c r="A74" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B74" s="18" t="s">
-        <v>398</v>
+      <c r="B74" s="16" t="s">
+        <v>392</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>149</v>
@@ -4053,8 +4036,8 @@
       <c r="R75" s="4"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A76" s="20" t="s">
-        <v>516</v>
+      <c r="A76" s="18" t="s">
+        <v>500</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -4075,7 +4058,7 @@
       <c r="R76" s="4"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B77" s="4" t="s">
@@ -4085,8 +4068,8 @@
       <c r="D77" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4" t="s">
         <v>70</v>
@@ -4103,7 +4086,7 @@
       <c r="R77" s="4"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -4111,7 +4094,7 @@
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="1" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -4283,31 +4266,31 @@
       <c r="R84" s="4"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A85" s="12"/>
+      <c r="A85" s="10"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
+      <c r="A92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
+      <c r="A93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="15"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A94" s="16"/>
-      <c r="D94" s="16"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
+      <c r="A94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
+      <c r="A95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4317,40 +4300,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4360,15 +4314,15 @@
     <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>67</v>
@@ -4478,7 +4432,7 @@
         <v>207</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4494,39 +4448,39 @@
         <v>211</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -4534,23 +4488,23 @@
         <v>212</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -4566,7 +4520,7 @@
         <v>216</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -4590,15 +4544,15 @@
         <v>218</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -20985,10 +20939,10 @@
     </row>
     <row r="37" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -37375,10 +37329,10 @@
     </row>
     <row r="38" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -53789,10 +53743,10 @@
     </row>
     <row r="43" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="45" spans="1:16384" x14ac:dyDescent="0.25">
@@ -53800,7 +53754,7 @@
         <v>219</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="46" spans="1:16384" x14ac:dyDescent="0.25">
@@ -53808,7 +53762,7 @@
         <v>220</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="47" spans="1:16384" x14ac:dyDescent="0.25">
@@ -53816,7 +53770,7 @@
         <v>221</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="1:16384" x14ac:dyDescent="0.25">
@@ -53824,23 +53778,23 @@
         <v>222</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -53880,7 +53834,7 @@
         <v>96</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -53944,7 +53898,7 @@
         <v>238</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -53952,279 +53906,1327 @@
         <v>245</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="27" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B111" s="1" t="s">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="J79" s="1" t="s">
         <v>404</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -54234,1413 +55236,110 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" customWidth="1"/>
-    <col min="8" max="8" width="44.85546875" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>151</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="C2" s="17"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I4" s="5"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="C4" s="17"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="I5" s="5"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="C5" s="17"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I6" s="5"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>491</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>492</v>
+      </c>
+      <c r="C6" s="17"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="J11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="J13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="J14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="J15" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="J16" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="J17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="J18" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="J19" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="J21" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="J22" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="J23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="J24" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="J25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="J27" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="J28" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="J30" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="J31" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="J32" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="J33" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="J34" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="J35" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="J36" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="J38" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="J40" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="J42" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="J43" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="J44" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="J46" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="J48" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="J49" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="J50" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="J52" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="E53" s="5"/>
-      <c r="J53" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="E54" s="5"/>
-      <c r="J54" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="E55" s="5"/>
-      <c r="J55" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="E56" s="5"/>
-      <c r="J56" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="J57" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="J58" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="J59" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="E61" s="5"/>
-      <c r="J61" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="E62" s="5"/>
-      <c r="J62" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="E63" s="5"/>
-      <c r="J63" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="J65" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J66" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E67" s="5"/>
-      <c r="J67" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E68" s="5"/>
-      <c r="J68" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="E70" s="5"/>
-      <c r="J70" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="E71" s="5"/>
-      <c r="J71" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="E72" s="5"/>
-      <c r="J72" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="E74" s="5"/>
-      <c r="J74" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>473</v>
-      </c>
-      <c r="E75" s="5"/>
-      <c r="J75" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="E76" s="5"/>
-      <c r="J76" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="E77" s="5"/>
-      <c r="J77" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="E78" s="5"/>
-      <c r="J78" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E80" s="5"/>
-      <c r="J80" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="E81" s="5"/>
-      <c r="J81" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="E82" s="5"/>
-      <c r="J82" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="E83" s="5"/>
-      <c r="J83" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="E85" s="5"/>
-      <c r="J85" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="E87" s="5"/>
-      <c r="J87" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="E88" s="5"/>
-      <c r="J88" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="E90" s="5"/>
-      <c r="J90" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="C91" s="5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="E91" s="5"/>
-      <c r="J91" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="C92" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>494</v>
-      </c>
-      <c r="E92" s="5"/>
-      <c r="J92" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="E93" s="5"/>
-      <c r="J93" t="s">
-        <v>410</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="17.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>503</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>504</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>505</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="13">
-        <v>0.6</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>506</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>507</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>508</v>
-      </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>510</v>
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed label for malnutrition_anemia
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1525,9 +1525,6 @@
     <t>label ear_end</t>
   </si>
   <si>
-    <t>label_malnut_anemia_end</t>
-  </si>
-  <si>
     <t>selected(data('cough'), 'no')</t>
   </si>
   <si>
@@ -1589,6 +1586,9 @@
   </si>
   <si>
     <t>{{calculates.med_danger_anemia() == "danger" &amp;&amp; !(calculates.low_danger_pneumonia() == "danger" || calculates.med_danger_dehydration() == "danger" || calculates.med_danger_ear() == "danger" || calculates.low_danger_dehydration() == "danger" || calculates.med_danger_diarrhea() == "danger" || calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger"|| calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger"  || calculates.med_danger_malaria() == "danger" || calculates.low_danger_malaria() == "danger") ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>label malnut_anemia_end</t>
   </si>
 </sst>
 </file>
@@ -2053,9 +2053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,11 +2684,11 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="19" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -2879,11 +2879,11 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -3215,11 +3215,11 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -4037,7 +4037,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>500</v>
+        <v>521</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -54190,7 +54190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
@@ -54449,7 +54449,7 @@
         <v>432</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -54460,7 +54460,7 @@
         <v>427</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>432</v>
@@ -54483,7 +54483,7 @@
         <v>432</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -54797,13 +54797,13 @@
         <v>236</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -54831,7 +54831,7 @@
         <v>251</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -54904,7 +54904,7 @@
         <v>412</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -54960,7 +54960,7 @@
         <v>425</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -55002,7 +55002,7 @@
         <v>256</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -55030,7 +55030,7 @@
         <v>256</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -55170,7 +55170,7 @@
         <v>475</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -55226,7 +55226,7 @@
         <v>480</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rest of summary/treatment in community
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bennett\workspace\cse481k\AdaptiveODK\form-files\adaptiveIMCI_community\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="calculates" sheetId="2" r:id="rId2"/>
+    <sheet name="calculates" sheetId="6" r:id="rId2"/>
     <sheet name="choices" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
     <sheet name="prompt_types" sheetId="5" r:id="rId5"/>
@@ -23,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="523">
   <si>
     <t>type</t>
   </si>
@@ -304,19 +299,10 @@
     <t>general_danger_level</t>
   </si>
   <si>
-    <t>calculates.has_cough()? "Present" : "Not present"</t>
-  </si>
-  <si>
     <t>diarrhea_danger_level</t>
   </si>
   <si>
-    <t>calculates.has_diarrhea()? "Present" : "Not present"</t>
-  </si>
-  <si>
     <t>ear_danger_level</t>
-  </si>
-  <si>
-    <t>calculates.has_fever()? "Present" : "Not present"</t>
   </si>
   <si>
     <t>malaria_measles_danger_level</t>
@@ -410,24 +396,6 @@
   </si>
   <si>
     <t>{{calculates.danger_class_pneumonia()}}</t>
-  </si>
-  <si>
-    <t>calculates.general_danger_level() == "Present" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>calculates.pneumonia_danger_level() == "Present" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>calculates.diarrhea_danger_level() == "Present" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>calculates.malaria_measles_danger_level() == "Present" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>calculates.ear_danger_level() == "Present" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>!calculates.can_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Present" : "Not present"</t>
   </si>
   <si>
     <t>cough</t>
@@ -605,9 +573,6 @@
   </si>
   <si>
     <t>danger_class_malnut_anemia</t>
-  </si>
-  <si>
-    <t>"TODO"</t>
   </si>
   <si>
     <t>malnut_anemia_danger_level</t>
@@ -811,9 +776,6 @@
     <t>selected(data('malaria_risk'), 'yes')</t>
   </si>
   <si>
-    <t>calculates .has_ear_problem() || calculates.has_ear_pain() || calculates.has_ear_discharge()? "Present" : "Not present"</t>
-  </si>
-  <si>
     <t>selected(data('fever_persistent', 'yes'))</t>
   </si>
   <si>
@@ -850,16 +812,10 @@
     <t>selected(data('measles_eyeclouding'), 'yes')</t>
   </si>
   <si>
-    <t>calculates.had_measles() &amp;&amp; (calculates.general_danger_level() == "Present" || calculates.has_eyeclouding() || calculates.has_ulcers())? "danger" : "good"</t>
-  </si>
-  <si>
     <t>calculates.had_measles() &amp;&amp; calculates.high_danger_measles() == "good" &amp;&amp; calculates.has_eyedischarge() ? "danger" : "good"</t>
   </si>
   <si>
     <t>calculates.had_measles() &amp;&amp; calculates.high_danger_measles() == "good" &amp;&amp; calculates.med_danger_measles() == "good" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>(calculates.has_fever() &amp;&amp; (calculates.has_stiffneck() || calculates.general_danger_level() == "Present") ) ? "danger" : "good"</t>
   </si>
   <si>
     <t>calculates.high_danger_malaria() == "good" &amp;&amp; (calculates.has_fever() &amp;&amp; calculates.malaria_risk()) || (calculates.has_fever() &amp;&amp; !calculates.malaria_risk() &amp;&amp; !calculates.has_rash_runnynose_redeyes() &amp;&amp; !calculates.had_measles()) ? "danger" : "good"</t>
@@ -1073,9 +1029,6 @@
   </si>
   <si>
     <t>calculates.has_cough() &amp;&amp; calculates.high_danger_pneumonia() == "good" &amp;&amp; calculates.has_fast_breathing() ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>calculates.has_cough() &amp;&amp; (calculates.general_danger_level() == "Present" || calculates.has_indrawing_stridor_wheezing()) ? "danger" : "good"</t>
   </si>
   <si>
     <t>selected(data('indraw_stridor_wheezing'), 'yes')</t>
@@ -1369,9 +1322,6 @@
     <t>severe_classification</t>
   </si>
   <si>
-    <t>calculates.general_danger_level() == "Present" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_malaria() == "danger"|| calculates.high_danger_measles() == "danger" || calculates.high_danger_ear() == "danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
-  </si>
-  <si>
     <t>Give frequent sips of ORS</t>
   </si>
   <si>
@@ -1483,9 +1433,6 @@
     <t>{{calculates.med_danger_malaria() == "danger" || calculates.med_danger_pneumonia() == "danger" || calculates.low_danger_pneumonia() == "danger"  || calculates.med_danger_malaria() == "danger" || calculates.low_danger_malaria() == "danger" || calculates.med_danger_dehydration() == "danger" || calculates.low_danger_dehydration() == "danger" || calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger" ? "danger" : "good"}}</t>
   </si>
   <si>
-    <t>calculates.general_danger_level() == "Present" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_ear() =="danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
-  </si>
-  <si>
     <t>adaptiveIMCI_commnunity</t>
   </si>
   <si>
@@ -1589,6 +1536,57 @@
   </si>
   <si>
     <t>label malnut_anemia_end</t>
+  </si>
+  <si>
+    <t>calculates.general_danger_level() == "Danger" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_malaria() == "danger"|| calculates.high_danger_measles() == "danger" || calculates.high_danger_ear() == "danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>!calculates.can_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Danger" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_pneumonia() == "danger" ? "Danger" : calculates.med_danger_pneumonia() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_diarrhea() == "danger" ? "Danger" :  calculates.med_danger_diarrhea() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" ? "Danger" :  calculates.med_danger_malaria() == "danger" || calculates.med_danger_measles() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates .high_danger_ear() == "danger" ? "Danger" :  calculates.med_danger_ear() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "Danger" : calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.general_danger_level() == "Danger" ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_pneumonia() == "danger" ? "danger" : calculates.med_danger_pneumonia() == "danger" ? "warning" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_diarrhea() == "danger" ? "danger" : calculates.med_danger_diarrhea() == "danger" ? "warning" : "good"</t>
+  </si>
+  <si>
+    <t>(calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger") ? "danger" : (calculates.med_danger_malaria() == "danger" || calculates.med_danger_measles() == "danger") ? "warning" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_ear() == "danger" ? "danger" : calculates.med_danger_ear() == "danger" ? "warning" : "good"</t>
+  </si>
+  <si>
+    <t>(calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger") ? "danger" : (calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger") ? "warning" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.general_danger_level() == "Danger" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_ear() =="danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>(calculates.has_fever() &amp;&amp; (calculates.has_stiffneck() || calculates.general_danger_level() == "Danger") ) ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.had_measles() &amp;&amp; (calculates.general_danger_level() == "Danger" || calculates.has_eyeclouding() || calculates.has_ulcers())? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.has_cough() &amp;&amp; (calculates.general_danger_level() == "Danger" || calculates.has_indrawing_stridor_wheezing()) ? "danger" : "good"</t>
   </si>
 </sst>
 </file>
@@ -2043,7 +2041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2053,7 +2051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
@@ -2083,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>1</v>
@@ -2095,7 +2093,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>14</v>
@@ -2134,12 +2132,12 @@
         <v>13</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2164,7 +2162,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2249,7 +2247,7 @@
         <v>44</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -2278,7 +2276,7 @@
         <v>46</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -2317,7 +2315,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2339,7 +2337,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2364,7 +2362,7 @@
         <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2396,7 +2394,7 @@
         <v>52</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G12" s="4" t="b">
         <v>1</v>
@@ -2426,7 +2424,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G13" s="4" t="b">
         <v>1</v>
@@ -2456,7 +2454,7 @@
         <v>47</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G14" s="4" t="b">
         <v>1</v>
@@ -2525,13 +2523,13 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G17" s="4" t="b">
         <v>1</v>
@@ -2561,7 +2559,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G18" s="4" t="b">
         <v>1</v>
@@ -2591,7 +2589,7 @@
         <v>58</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G19" s="4" t="b">
         <v>1</v>
@@ -2621,7 +2619,7 @@
         <v>34</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G20" s="4" t="b">
         <v>1</v>
@@ -2662,7 +2660,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2684,11 +2682,11 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="19" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -2708,7 +2706,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2733,7 +2731,7 @@
         <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="9"/>
@@ -2753,18 +2751,18 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="13"/>
       <c r="D26" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -2781,15 +2779,15 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="13"/>
       <c r="D27" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -2812,13 +2810,13 @@
       <c r="B28" s="4"/>
       <c r="C28" s="13"/>
       <c r="D28" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -2857,7 +2855,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="13"/>
@@ -2879,11 +2877,11 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="1" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2903,7 +2901,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B32" s="4"/>
       <c r="D32" s="4"/>
@@ -2927,7 +2925,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2947,18 +2945,18 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="13"/>
       <c r="D34" s="1" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -2980,13 +2978,13 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -3008,13 +3006,13 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -3036,13 +3034,13 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -3064,13 +3062,13 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -3092,13 +3090,13 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -3120,13 +3118,13 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="1" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -3148,13 +3146,13 @@
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -3193,7 +3191,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3215,11 +3213,11 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="1" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -3239,7 +3237,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B45" s="4"/>
       <c r="D45" s="4"/>
@@ -3263,7 +3261,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -3288,13 +3286,13 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
@@ -3311,18 +3309,18 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="13"/>
       <c r="D48" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -3344,13 +3342,13 @@
       <c r="B49" s="4"/>
       <c r="C49" s="13"/>
       <c r="D49" s="4" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -3372,13 +3370,13 @@
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -3400,13 +3398,13 @@
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -3428,13 +3426,13 @@
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -3476,10 +3474,10 @@
         <v>43</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -3504,13 +3502,13 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -3532,13 +3530,13 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -3560,13 +3558,13 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
@@ -3605,7 +3603,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3627,7 +3625,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3652,7 +3650,7 @@
         <v>43</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -3683,7 +3681,7 @@
         <v>60</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -3711,7 +3709,7 @@
         <v>62</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
@@ -3733,13 +3731,13 @@
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -3767,7 +3765,7 @@
         <v>64</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
@@ -3806,7 +3804,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3828,7 +3826,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3853,7 +3851,7 @@
         <v>43</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -3878,13 +3876,13 @@
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
@@ -3906,13 +3904,13 @@
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -3934,13 +3932,13 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
@@ -3962,13 +3960,13 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
@@ -3988,17 +3986,17 @@
         <v>24</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -4037,7 +4035,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -4062,7 +4060,7 @@
         <v>31</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4" t="s">
@@ -4090,11 +4088,11 @@
         <v>43</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="1" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -4113,15 +4111,15 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -4139,15 +4137,15 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -4165,12 +4163,12 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="4"/>
@@ -4187,20 +4185,20 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
       <c r="S81" s="3" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -4218,12 +4216,12 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="1" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="4"/>
@@ -4240,7 +4238,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
       <c r="S83" s="3" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
@@ -4303,8 +4301,8 @@
   <dimension ref="A1:XFD111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4341,10 +4339,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4413,114 +4411,114 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -4528,31 +4526,31 @@
         <v>77</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -20939,10 +20937,10 @@
     </row>
     <row r="37" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -37329,10 +37327,10 @@
     </row>
     <row r="38" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -53743,58 +53741,58 @@
     </row>
     <row r="43" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="46" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="47" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="48" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>448</v>
+        <v>506</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -53802,383 +53800,383 @@
         <v>92</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>134</v>
+        <v>507</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>93</v>
+        <v>508</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>95</v>
+        <v>509</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>97</v>
+        <v>510</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>262</v>
+        <v>511</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>194</v>
+        <v>512</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>513</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>130</v>
+        <v>514</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>131</v>
+        <v>515</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>132</v>
+        <v>516</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>133</v>
+        <v>517</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>194</v>
+        <v>518</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>486</v>
+        <v>519</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>278</v>
+        <v>520</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>275</v>
+        <v>521</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>350</v>
+        <v>522</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -54190,7 +54188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
@@ -54219,25 +54217,25 @@
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -54268,22 +54266,22 @@
         <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -54291,22 +54289,22 @@
         <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -54314,22 +54312,22 @@
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -54337,22 +54335,22 @@
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -54360,22 +54358,22 @@
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -54383,850 +54381,850 @@
         <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>514</v>
+        <v>498</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -55264,16 +55262,16 @@
         <v>17</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>488</v>
+        <v>472</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
       <c r="C3" s="17"/>
     </row>
@@ -55291,25 +55289,25 @@
         <v>19</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="C5" s="17"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed 'Danger' label to 'Present'
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bennett\workspace\cse481k\AdaptiveODK\form-files\adaptiveIMCI_community\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9570" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1538,30 +1543,6 @@
     <t>label malnut_anemia_end</t>
   </si>
   <si>
-    <t>calculates.general_danger_level() == "Danger" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_malaria() == "danger"|| calculates.high_danger_measles() == "danger" || calculates.high_danger_ear() == "danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>!calculates.can_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Danger" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_pneumonia() == "danger" ? "Danger" : calculates.med_danger_pneumonia() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_diarrhea() == "danger" ? "Danger" :  calculates.med_danger_diarrhea() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" ? "Danger" :  calculates.med_danger_malaria() == "danger" || calculates.med_danger_measles() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates .high_danger_ear() == "danger" ? "Danger" :  calculates.med_danger_ear() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "Danger" : calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.general_danger_level() == "Danger" ? "danger" : "good"</t>
-  </si>
-  <si>
     <t>calculates.high_danger_pneumonia() == "danger" ? "danger" : calculates.med_danger_pneumonia() == "danger" ? "warning" : "good"</t>
   </si>
   <si>
@@ -1577,16 +1558,40 @@
     <t>(calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger") ? "danger" : (calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger") ? "warning" : "good"</t>
   </si>
   <si>
-    <t>calculates.general_danger_level() == "Danger" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_ear() =="danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
+    <t>calculates.general_danger_level() == "Present" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_malaria() == "danger"|| calculates.high_danger_measles() == "danger" || calculates.high_danger_ear() == "danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
   </si>
   <si>
-    <t>(calculates.has_fever() &amp;&amp; (calculates.has_stiffneck() || calculates.general_danger_level() == "Danger") ) ? "danger" : "good"</t>
+    <t>!calculates.can_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Present" : "Not present"</t>
   </si>
   <si>
-    <t>calculates.had_measles() &amp;&amp; (calculates.general_danger_level() == "Danger" || calculates.has_eyeclouding() || calculates.has_ulcers())? "danger" : "good"</t>
+    <t>calculates.high_danger_pneumonia() == "danger" ? "Present" : calculates.med_danger_pneumonia() == "danger" ? "Present" : "Not present"</t>
   </si>
   <si>
-    <t>calculates.has_cough() &amp;&amp; (calculates.general_danger_level() == "Danger" || calculates.has_indrawing_stridor_wheezing()) ? "danger" : "good"</t>
+    <t>calculates.high_danger_diarrhea() == "danger" ? "Present" :  calculates.med_danger_diarrhea() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" ? "Present" :  calculates.med_danger_malaria() == "danger" || calculates.med_danger_measles() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates .high_danger_ear() == "danger" ? "Present" :  calculates.med_danger_ear() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "Present" : calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger" ? "Present" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.general_danger_level() == "Present" ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.general_danger_level() == "Present" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_ear() =="danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>(calculates.has_fever() &amp;&amp; (calculates.has_stiffneck() || calculates.general_danger_level() == "Present") ) ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.had_measles() &amp;&amp; (calculates.general_danger_level() == "Present" || calculates.has_eyeclouding() || calculates.has_ulcers())? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.has_cough() &amp;&amp; (calculates.general_danger_level() == "Present" || calculates.has_indrawing_stridor_wheezing()) ? "danger" : "good"</t>
   </si>
 </sst>
 </file>
@@ -2041,7 +2046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2052,31 +2057,31 @@
   <dimension ref="A1:S95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="41" style="3" customWidth="1"/>
     <col min="6" max="6" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="3"/>
-    <col min="8" max="8" width="20.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="3" customWidth="1"/>
-    <col min="10" max="12" width="8.85546875" style="3"/>
-    <col min="13" max="13" width="17.28515625" style="3" customWidth="1"/>
-    <col min="14" max="15" width="8.85546875" style="3"/>
-    <col min="16" max="16" width="17.42578125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="3"/>
+    <col min="7" max="7" width="8.88671875" style="3"/>
+    <col min="8" max="8" width="20.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" style="3" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="3"/>
+    <col min="13" max="13" width="17.33203125" style="3" customWidth="1"/>
+    <col min="14" max="15" width="8.88671875" style="3"/>
+    <col min="16" max="16" width="17.44140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="19.88671875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="21.5546875" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2135,7 +2140,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>131</v>
       </c>
@@ -2157,7 +2162,7 @@
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -2181,7 +2186,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
@@ -2209,7 +2214,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -2237,7 +2242,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -2263,7 +2268,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -2291,7 +2296,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -2313,7 +2318,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>482</v>
       </c>
@@ -2335,7 +2340,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>141</v>
       </c>
@@ -2357,7 +2362,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -2381,7 +2386,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -2411,7 +2416,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -2441,7 +2446,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -2471,7 +2476,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>48</v>
       </c>
@@ -2493,7 +2498,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>43</v>
       </c>
@@ -2517,7 +2522,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
@@ -2546,7 +2551,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -2576,7 +2581,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
@@ -2606,7 +2611,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -2636,7 +2641,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -2658,7 +2663,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>479</v>
       </c>
@@ -2680,7 +2685,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>487</v>
       </c>
@@ -2704,7 +2709,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>133</v>
       </c>
@@ -2726,7 +2731,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>43</v>
       </c>
@@ -2749,7 +2754,7 @@
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>143</v>
       </c>
@@ -2777,7 +2782,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>143</v>
       </c>
@@ -2803,7 +2808,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
@@ -2831,7 +2836,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
@@ -2853,7 +2858,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>480</v>
       </c>
@@ -2875,7 +2880,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>488</v>
       </c>
@@ -2899,7 +2904,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>147</v>
       </c>
@@ -2920,7 +2925,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>43</v>
       </c>
@@ -2943,7 +2948,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>143</v>
       </c>
@@ -2971,7 +2976,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>24</v>
       </c>
@@ -2999,7 +3004,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -3027,7 +3032,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>24</v>
       </c>
@@ -3055,7 +3060,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
@@ -3083,7 +3088,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -3111,7 +3116,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -3139,7 +3144,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>24</v>
       </c>
@@ -3167,7 +3172,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>48</v>
       </c>
@@ -3189,7 +3194,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
         <v>481</v>
       </c>
@@ -3211,7 +3216,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
         <v>489</v>
       </c>
@@ -3235,7 +3240,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>187</v>
       </c>
@@ -3256,7 +3261,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>43</v>
       </c>
@@ -3279,7 +3284,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
@@ -3307,7 +3312,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>143</v>
       </c>
@@ -3335,7 +3340,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>24</v>
       </c>
@@ -3363,7 +3368,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>24</v>
       </c>
@@ -3391,7 +3396,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>24</v>
       </c>
@@ -3419,7 +3424,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>24</v>
       </c>
@@ -3447,7 +3452,7 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>48</v>
       </c>
@@ -3469,7 +3474,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>43</v>
       </c>
@@ -3495,7 +3500,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>24</v>
       </c>
@@ -3523,7 +3528,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>24</v>
       </c>
@@ -3551,7 +3556,7 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>24</v>
       </c>
@@ -3579,7 +3584,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>48</v>
       </c>
@@ -3601,7 +3606,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="18" t="s">
         <v>490</v>
       </c>
@@ -3623,7 +3628,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>134</v>
       </c>
@@ -3645,7 +3650,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>43</v>
       </c>
@@ -3668,7 +3673,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>24</v>
       </c>
@@ -3696,7 +3701,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>24</v>
       </c>
@@ -3724,7 +3729,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>24</v>
       </c>
@@ -3752,7 +3757,7 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>24</v>
       </c>
@@ -3780,7 +3785,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>48</v>
       </c>
@@ -3802,7 +3807,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
         <v>483</v>
       </c>
@@ -3824,7 +3829,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>182</v>
       </c>
@@ -3846,7 +3851,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>43</v>
       </c>
@@ -3869,7 +3874,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>24</v>
       </c>
@@ -3897,7 +3902,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>24</v>
       </c>
@@ -3925,7 +3930,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>24</v>
       </c>
@@ -3953,7 +3958,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>24</v>
       </c>
@@ -3981,7 +3986,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>24</v>
       </c>
@@ -4011,7 +4016,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>48</v>
       </c>
@@ -4033,7 +4038,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="18" t="s">
         <v>505</v>
       </c>
@@ -4055,7 +4060,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
         <v>31</v>
       </c>
@@ -4083,7 +4088,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
         <v>43</v>
       </c>
@@ -4109,7 +4114,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>214</v>
       </c>
@@ -4135,7 +4140,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>214</v>
       </c>
@@ -4161,7 +4166,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>219</v>
       </c>
@@ -4188,7 +4193,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>214</v>
       </c>
@@ -4214,7 +4219,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>225</v>
       </c>
@@ -4241,7 +4246,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>48</v>
       </c>
@@ -4263,28 +4268,28 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="14"/>
       <c r="D92" s="14"/>
       <c r="E92" s="15"/>
       <c r="F92" s="15"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="14"/>
       <c r="D93" s="14"/>
       <c r="E93" s="15"/>
       <c r="F93" s="15"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="14"/>
       <c r="D94" s="14"/>
       <c r="E94" s="15"/>
       <c r="F94" s="15"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="14"/>
       <c r="D95" s="14"/>
       <c r="E95" s="15"/>
@@ -4300,19 +4305,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
-    <col min="2" max="2" width="97.42578125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="97.44140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -4320,8 +4325,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -4329,7 +4334,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
@@ -4337,7 +4342,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>189</v>
       </c>
@@ -4345,7 +4350,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
@@ -4353,7 +4358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
@@ -4361,7 +4366,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -4369,7 +4374,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
@@ -4377,7 +4382,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
@@ -4385,7 +4390,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -4393,7 +4398,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -4401,7 +4406,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -4409,7 +4414,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>191</v>
       </c>
@@ -4417,7 +4422,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>194</v>
       </c>
@@ -4425,7 +4430,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>197</v>
       </c>
@@ -4433,7 +4438,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>199</v>
       </c>
@@ -4441,7 +4446,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>201</v>
       </c>
@@ -4449,7 +4454,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>297</v>
       </c>
@@ -4457,7 +4462,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>298</v>
       </c>
@@ -4465,7 +4470,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>299</v>
       </c>
@@ -4473,7 +4478,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>300</v>
       </c>
@@ -4481,7 +4486,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>202</v>
       </c>
@@ -4489,7 +4494,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>308</v>
       </c>
@@ -4497,7 +4502,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>250</v>
       </c>
@@ -4505,7 +4510,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>204</v>
       </c>
@@ -4513,7 +4518,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>206</v>
       </c>
@@ -4521,7 +4526,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
@@ -4529,7 +4534,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>207</v>
       </c>
@@ -4537,7 +4542,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>208</v>
       </c>
@@ -4545,7 +4550,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="36" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>258</v>
       </c>
@@ -20935,7 +20940,7 @@
       <c r="XFC36" s="4"/>
       <c r="XFD36" s="4"/>
     </row>
-    <row r="37" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>259</v>
       </c>
@@ -37325,7 +37330,7 @@
       <c r="XFC37" s="4"/>
       <c r="XFD37" s="4"/>
     </row>
-    <row r="38" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>260</v>
       </c>
@@ -53715,7 +53720,7 @@
       <c r="XFC38" s="4"/>
       <c r="XFD38" s="4"/>
     </row>
-    <row r="40" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
@@ -53723,7 +53728,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
@@ -53731,7 +53736,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -53739,7 +53744,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>313</v>
       </c>
@@ -53747,7 +53752,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="45" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>209</v>
       </c>
@@ -53755,7 +53760,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>210</v>
       </c>
@@ -53763,7 +53768,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="47" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>211</v>
       </c>
@@ -53771,7 +53776,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="48" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>212</v>
       </c>
@@ -53779,7 +53784,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>379</v>
       </c>
@@ -53787,111 +53792,111 @@
         <v>380</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>433</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>184</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>228</v>
       </c>
@@ -53899,7 +53904,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>235</v>
       </c>
@@ -53907,7 +53912,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>248</v>
       </c>
@@ -53915,7 +53920,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>275</v>
       </c>
@@ -53923,7 +53928,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>254</v>
       </c>
@@ -53931,7 +53936,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>255</v>
       </c>
@@ -53939,7 +53944,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>256</v>
       </c>
@@ -53947,7 +53952,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>286</v>
       </c>
@@ -53955,7 +53960,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>276</v>
       </c>
@@ -53963,7 +53968,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>277</v>
       </c>
@@ -53971,7 +53976,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>278</v>
       </c>
@@ -53979,7 +53984,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>349</v>
       </c>
@@ -53987,7 +53992,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>351</v>
       </c>
@@ -53995,7 +54000,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>353</v>
       </c>
@@ -54003,7 +54008,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>355</v>
       </c>
@@ -54011,7 +54016,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>357</v>
       </c>
@@ -54019,7 +54024,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>359</v>
       </c>
@@ -54027,7 +54032,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>361</v>
       </c>
@@ -54035,7 +54040,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>362</v>
       </c>
@@ -54043,7 +54048,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>363</v>
       </c>
@@ -54051,7 +54056,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>364</v>
       </c>
@@ -54059,7 +54064,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>357</v>
       </c>
@@ -54067,7 +54072,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>365</v>
       </c>
@@ -54075,7 +54080,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>288</v>
       </c>
@@ -54083,7 +54088,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>305</v>
       </c>
@@ -54091,7 +54096,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>309</v>
       </c>
@@ -54099,7 +54104,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>279</v>
       </c>
@@ -54107,7 +54112,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>280</v>
       </c>
@@ -54115,7 +54120,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>310</v>
       </c>
@@ -54123,7 +54128,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>281</v>
       </c>
@@ -54131,7 +54136,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>282</v>
       </c>
@@ -54139,7 +54144,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>283</v>
       </c>
@@ -54147,7 +54152,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>284</v>
       </c>
@@ -54155,7 +54160,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>285</v>
       </c>
@@ -54163,7 +54168,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>381</v>
       </c>
@@ -54171,7 +54176,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>382</v>
       </c>
@@ -54188,25 +54193,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="27" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="31.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -54238,7 +54243,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -54250,7 +54255,7 @@
       </c>
       <c r="I2" s="21"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -54261,7 +54266,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -54284,7 +54289,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -54307,7 +54312,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -54330,7 +54335,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -54353,7 +54358,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -54376,7 +54381,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -54399,7 +54404,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>226</v>
       </c>
@@ -54416,7 +54421,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>226</v>
       </c>
@@ -54433,7 +54438,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>226</v>
       </c>
@@ -54450,7 +54455,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>226</v>
       </c>
@@ -54467,7 +54472,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>226</v>
       </c>
@@ -54484,7 +54489,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>226</v>
       </c>
@@ -54501,7 +54506,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>226</v>
       </c>
@@ -54518,7 +54523,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>226</v>
       </c>
@@ -54535,7 +54540,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>226</v>
       </c>
@@ -54552,7 +54557,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>226</v>
       </c>
@@ -54569,7 +54574,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>226</v>
       </c>
@@ -54586,7 +54591,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>226</v>
       </c>
@@ -54603,7 +54608,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>226</v>
       </c>
@@ -54620,7 +54625,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>226</v>
       </c>
@@ -54637,7 +54642,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>226</v>
       </c>
@@ -54654,7 +54659,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>226</v>
       </c>
@@ -54671,7 +54676,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>226</v>
       </c>
@@ -54688,7 +54693,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>226</v>
       </c>
@@ -54705,7 +54710,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>226</v>
       </c>
@@ -54722,7 +54727,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>226</v>
       </c>
@@ -54739,7 +54744,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>226</v>
       </c>
@@ -54756,7 +54761,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>226</v>
       </c>
@@ -54773,7 +54778,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>226</v>
       </c>
@@ -54790,7 +54795,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>226</v>
       </c>
@@ -54804,7 +54809,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>233</v>
       </c>
@@ -54818,7 +54823,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>233</v>
       </c>
@@ -54832,7 +54837,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>233</v>
       </c>
@@ -54846,7 +54851,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>233</v>
       </c>
@@ -54863,7 +54868,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>233</v>
       </c>
@@ -54877,7 +54882,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>233</v>
       </c>
@@ -54891,7 +54896,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>233</v>
       </c>
@@ -54905,7 +54910,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>233</v>
       </c>
@@ -54919,7 +54924,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>233</v>
       </c>
@@ -54933,7 +54938,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>233</v>
       </c>
@@ -54947,7 +54952,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>233</v>
       </c>
@@ -54961,7 +54966,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>233</v>
       </c>
@@ -54975,7 +54980,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>233</v>
       </c>
@@ -54989,7 +54994,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>233</v>
       </c>
@@ -55003,7 +55008,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>233</v>
       </c>
@@ -55017,7 +55022,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>233</v>
       </c>
@@ -55031,7 +55036,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>233</v>
       </c>
@@ -55045,7 +55050,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>233</v>
       </c>
@@ -55059,7 +55064,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>233</v>
       </c>
@@ -55073,7 +55078,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>233</v>
       </c>
@@ -55087,7 +55092,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>233</v>
       </c>
@@ -55101,7 +55106,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>233</v>
       </c>
@@ -55115,7 +55120,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>451</v>
       </c>
@@ -55129,7 +55134,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>451</v>
       </c>
@@ -55143,7 +55148,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>233</v>
       </c>
@@ -55157,7 +55162,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>233</v>
       </c>
@@ -55171,7 +55176,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>233</v>
       </c>
@@ -55185,7 +55190,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>233</v>
       </c>
@@ -55199,7 +55204,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>233</v>
       </c>
@@ -55213,7 +55218,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>233</v>
       </c>
@@ -55241,14 +55246,14 @@
       <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" style="4" customWidth="1"/>
     <col min="2" max="2" width="24" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="4"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -55257,7 +55262,7 @@
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -55266,7 +55271,7 @@
       </c>
       <c r="C2" s="17"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>472</v>
       </c>
@@ -55275,7 +55280,7 @@
       </c>
       <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -55284,7 +55289,7 @@
       </c>
       <c r="C4" s="17"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -55293,7 +55298,7 @@
       </c>
       <c r="C5" s="17"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>475</v>
       </c>
@@ -55302,7 +55307,7 @@
       </c>
       <c r="C6" s="17"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>477</v>
       </c>
@@ -55325,14 +55330,14 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="17.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
updated forms with three levels (severe, moderate, not present)
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9570" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="20730" windowHeight="9390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1553,24 +1553,6 @@
     <t>(calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger") ? "danger" : (calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger") ? "warning" : "good"</t>
   </si>
   <si>
-    <t>calculates.general_danger_level() == "Present" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_malaria() == "danger"|| calculates.high_danger_measles() == "danger" || calculates.high_danger_ear() == "danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_pneumonia() == "danger" ? "Present" : calculates.med_danger_pneumonia() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_diarrhea() == "danger" ? "Present" :  calculates.med_danger_diarrhea() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" ? "Present" :  calculates.med_danger_malaria() == "danger" || calculates.med_danger_measles() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates .high_danger_ear() == "danger" ? "Present" :  calculates.med_danger_ear() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
-    <t>calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "Present" : calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger" ? "Present" : "Not present"</t>
-  </si>
-  <si>
     <t>calculates.general_danger_level() == "Present" ? "danger" : "good"</t>
   </si>
   <si>
@@ -1586,13 +1568,31 @@
     <t>calculates.has_cough() &amp;&amp; (calculates.general_danger_level() == "Present" || calculates.has_indrawing_stridor_wheezing()) ? "danger" : "good"</t>
   </si>
   <si>
-    <t>calculates.cannot_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Present" : "Not present"</t>
-  </si>
-  <si>
     <t>cannot_drink</t>
   </si>
   <si>
     <t>selected(data('drink'),'no')</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_malaria() == "danger" || calculates.high_danger_measles() == "danger" ? "Severe" :  calculates.med_danger_malaria() == "danger" || calculates.med_danger_measles() == "danger" ? "Moderate" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates .high_danger_ear() == "danger" ? "Severe" :  calculates.med_danger_ear() == "danger" ? "Moderate" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "Severe" : calculates.med_danger_malnut() == "danger" || calculates.med_danger_anemia() == "danger" ? "Moderate" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.general_danger_level() == "Severe" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_malaria() == "danger"|| calculates.high_danger_measles() == "danger" || calculates.high_danger_ear() == "danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
+  </si>
+  <si>
+    <t>calculates.cannot_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Severe" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_pneumonia() == "danger" ? "Severe" : calculates.med_danger_pneumonia() == "danger" ? "Moderate" : "Not present"</t>
+  </si>
+  <si>
+    <t>calculates.high_danger_diarrhea() == "danger" ? "Severe" :  calculates.med_danger_diarrhea() == "danger" ? "Moderate" : "Not present"</t>
   </si>
 </sst>
 </file>
@@ -2047,7 +2047,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2058,8 +2058,8 @@
   <dimension ref="A1:S95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4306,9 +4306,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4362,10 +4362,10 @@
     <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
@@ -4544,7 +4544,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="34" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>207</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>208</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="37" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>258</v>
       </c>
@@ -20950,7 +20950,7 @@
       <c r="XFC37" s="4"/>
       <c r="XFD37" s="4"/>
     </row>
-    <row r="38" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>259</v>
       </c>
@@ -37340,7 +37340,7 @@
       <c r="XFC38" s="4"/>
       <c r="XFD38" s="4"/>
     </row>
-    <row r="39" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>260</v>
       </c>
@@ -53730,7 +53730,7 @@
       <c r="XFC39" s="4"/>
       <c r="XFD39" s="4"/>
     </row>
-    <row r="41" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>79</v>
       </c>
@@ -53738,7 +53738,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>81</v>
       </c>
@@ -53746,7 +53746,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
@@ -53754,7 +53754,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>313</v>
       </c>
@@ -53762,7 +53762,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="46" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>209</v>
       </c>
@@ -53770,7 +53770,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="47" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>210</v>
       </c>
@@ -53778,7 +53778,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="48" spans="1:16384" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>211</v>
       </c>
@@ -53786,7 +53786,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>212</v>
       </c>
@@ -53794,7 +53794,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>379</v>
       </c>
@@ -53802,15 +53802,15 @@
         <v>380</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>433</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>92</v>
       </c>
@@ -53818,55 +53818,55 @@
         <v>522</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>512</v>
+        <v>523</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>97</v>
       </c>
@@ -53874,7 +53874,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>99</v>
       </c>
@@ -53911,7 +53911,7 @@
         <v>228</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -53919,7 +53919,7 @@
         <v>235</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -53930,7 +53930,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>275</v>
       </c>
@@ -53943,7 +53943,7 @@
         <v>254</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -53954,7 +53954,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>256</v>
       </c>
@@ -53975,7 +53975,7 @@
         <v>276</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -53986,7 +53986,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>278</v>
       </c>
@@ -54034,7 +54034,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>359</v>
       </c>
@@ -54082,7 +54082,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>365</v>
       </c>
@@ -54122,7 +54122,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>280</v>
       </c>
@@ -54130,7 +54130,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>310</v>
       </c>
@@ -54154,7 +54154,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>283</v>
       </c>
@@ -54170,7 +54170,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>285</v>
       </c>
@@ -54204,8 +54204,8 @@
   <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54703,7 +54703,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>226</v>
       </c>
@@ -54720,7 +54720,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>226</v>
       </c>
@@ -54737,7 +54737,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>226</v>
       </c>
@@ -54754,7 +54754,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>226</v>
       </c>
@@ -54771,7 +54771,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>226</v>
       </c>
@@ -54788,7 +54788,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>226</v>
       </c>
@@ -54805,7 +54805,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>226</v>
       </c>
@@ -54819,7 +54819,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>233</v>
       </c>
@@ -54833,7 +54833,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>233</v>
       </c>
@@ -54847,7 +54847,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>233</v>
       </c>
@@ -54861,7 +54861,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>233</v>
       </c>
@@ -54878,7 +54878,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>233</v>
       </c>
@@ -54892,7 +54892,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>233</v>
       </c>
@@ -54906,7 +54906,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>233</v>
       </c>
@@ -55251,9 +55251,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
re-enabled QR generation in community form
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_community/community.xlsx
+++ b/form-files/adaptiveIMCI_community/community.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="534">
   <si>
     <t>type</t>
   </si>
@@ -1617,6 +1617,15 @@
   <si>
     <t>data('fever_days') &gt; 0</t>
   </si>
+  <si>
+    <t>generate_qr</t>
+  </si>
+  <si>
+    <t>Finish Survey</t>
+  </si>
+  <si>
+    <t>generate_qr_code</t>
+  </si>
 </sst>
 </file>
 
@@ -2081,8 +2090,8 @@
   <dimension ref="A1:S95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4317,7 +4326,15 @@
       <c r="R84" s="4"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A85" s="10"/>
+      <c r="A85" t="s">
+        <v>531</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="14"/>

</xml_diff>